<commit_message>
My second commit on test data change
</commit_message>
<xml_diff>
--- a/src/main/java/com/lampenwelt/qa/testdata/TestData.xlsx
+++ b/src/main/java/com/lampenwelt/qa/testdata/TestData.xlsx
@@ -162,9 +162,6 @@
     <t>TotalAmountAfterAdd</t>
   </si>
   <si>
-    <t>301,60 €</t>
-  </si>
-  <si>
     <t>ItemPriceBeforeUpdate</t>
   </si>
   <si>
@@ -175,6 +172,9 @@
   </si>
   <si>
     <t>53,80 €</t>
+  </si>
+  <si>
+    <t>311,60 €</t>
   </si>
 </sst>
 </file>
@@ -497,7 +497,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -553,7 +553,7 @@
         <v>1</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>3</v>
@@ -568,7 +568,7 @@
         <v>5</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>6</v>
@@ -606,7 +606,7 @@
         <v>10</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>12</v>
@@ -621,7 +621,7 @@
         <v>11</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>13</v>
@@ -750,7 +750,7 @@
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -859,13 +859,13 @@
         <v>12</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="P2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
my second commit on cloud testing
</commit_message>
<xml_diff>
--- a/src/main/java/com/lampenwelt/qa/testdata/TestData.xlsx
+++ b/src/main/java/com/lampenwelt/qa/testdata/TestData.xlsx
@@ -174,7 +174,7 @@
     <t>53,80 €</t>
   </si>
   <si>
-    <t>311,60 €</t>
+    <t>321,60 €</t>
   </si>
 </sst>
 </file>
@@ -497,7 +497,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -750,7 +750,7 @@
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>

</xml_diff>